<commit_message>
PluginManager überarbeitet & WebLibrary hinzugefügt
</commit_message>
<xml_diff>
--- a/WebServer/Zeiterfassung.xlsx
+++ b/WebServer/Zeiterfassung.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\SWE1\WebServer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tplac_000\Documents\Visual Studio 2012\Projects\SWE1\WebServer\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
   <si>
     <t>Zeiterfassung</t>
   </si>
@@ -78,7 +78,10 @@
     <t>SensorCloud -Thread &amp; Timer</t>
   </si>
   <si>
-    <t>Url vervollständigt</t>
+    <t>WebServer - URL umgebaut, Response umgebaut</t>
+  </si>
+  <si>
+    <t>WebServer - Url vervollständigt</t>
   </si>
 </sst>
 </file>
@@ -459,7 +462,7 @@
   <dimension ref="A1:E158"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="A17" sqref="A17:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -700,15 +703,23 @@
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="5">
+        <v>41606</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="2">
+        <v>3</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="2"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>

</xml_diff>

<commit_message>
UnitTests & SensorCloud xml
</commit_message>
<xml_diff>
--- a/WebServer/Zeiterfassung.xlsx
+++ b/WebServer/Zeiterfassung.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="27">
   <si>
     <t>Zeiterfassung</t>
   </si>
@@ -93,7 +93,13 @@
     <t>StaticFile - Begonnen</t>
   </si>
   <si>
-    <t>WebServer - Plugin Manager, 1. UnitTest</t>
+    <t>WebServer - Plugin Manager, UnitTest - 1</t>
+  </si>
+  <si>
+    <t>UnitTest - 2, 3, 4</t>
+  </si>
+  <si>
+    <t>StaticFile - Fertig, SensorCloud - XML</t>
   </si>
 </sst>
 </file>
@@ -560,7 +566,7 @@
   <dimension ref="A1:E161"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -601,7 +607,7 @@
       </c>
       <c r="C4" s="13">
         <f>SUMIF(B8:B100,"Teresa",D8:D100)</f>
-        <v>37</v>
+        <v>39.5</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="3"/>
@@ -876,7 +882,7 @@
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="2">
-        <v>4</v>
+        <v>2.5</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>23</v>
@@ -898,18 +904,34 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="2"/>
-      <c r="B25" s="1"/>
+      <c r="A25" s="5">
+        <v>41611</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="C25" s="1"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="1"/>
+      <c r="D25" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="26" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="2"/>
-      <c r="B26" s="1"/>
+      <c r="A26" s="5">
+        <v>41611</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="C26" s="1"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="1"/>
+      <c r="D26" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="27" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>

</xml_diff>

<commit_message>
Esoterik Plugin beendet (Text fehlt noch)
</commit_message>
<xml_diff>
--- a/WebServer/Zeiterfassung.xlsx
+++ b/WebServer/Zeiterfassung.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\SWE1\WebServer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Teresa\Documents\Visual Studio 2012\Projects\WebServer\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="30">
   <si>
     <t>Zeiterfassung</t>
   </si>
@@ -103,6 +103,12 @@
   </si>
   <si>
     <t>Webserver - index.html Startseite</t>
+  </si>
+  <si>
+    <t>Navi &amp; Esoterik - begonnen</t>
+  </si>
+  <si>
+    <t>Esoterik - (fast) abgeschlossen</t>
   </si>
 </sst>
 </file>
@@ -568,8 +574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -610,7 +616,7 @@
       </c>
       <c r="C4" s="13">
         <f>SUMIF(B8:B100,"Teresa",D8:D100)</f>
-        <v>39.5</v>
+        <v>44</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="3"/>
@@ -952,18 +958,34 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="2"/>
-      <c r="B28" s="1"/>
+      <c r="A28" s="5">
+        <v>41633</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="C28" s="1"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="1"/>
+      <c r="D28" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="29" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="2"/>
-      <c r="B29" s="1"/>
+      <c r="A29" s="5">
+        <v>41635</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="C29" s="1"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="1"/>
+      <c r="D29" s="2">
+        <v>3</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="30" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>

</xml_diff>

<commit_message>
POST & GET - Fehler behoben
</commit_message>
<xml_diff>
--- a/WebServer/Zeiterfassung.xlsx
+++ b/WebServer/Zeiterfassung.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Teresa\Documents\Visual Studio 2012\Projects\WebServer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Teresa\Documents\Visual Studio 2012\Projects\SWE1\WebServer\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="33">
   <si>
     <t>Zeiterfassung</t>
   </si>
@@ -109,6 +109,15 @@
   </si>
   <si>
     <t>Esoterik - (fast) abgeschlossen</t>
+  </si>
+  <si>
+    <t>Esoterik - fertig</t>
+  </si>
+  <si>
+    <t>Webserver - post/get</t>
+  </si>
+  <si>
+    <t>Webserver - post/get &amp; Fehler behoben</t>
   </si>
 </sst>
 </file>
@@ -574,8 +583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -616,7 +625,7 @@
       </c>
       <c r="C4" s="13">
         <f>SUMIF(B8:B100,"Teresa",D8:D100)</f>
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="3"/>
@@ -988,25 +997,49 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="2"/>
-      <c r="B30" s="1"/>
+      <c r="A30" s="5">
+        <v>41636</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="C30" s="1"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="1"/>
+      <c r="D30" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="31" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="2"/>
-      <c r="B31" s="1"/>
+      <c r="A31" s="5">
+        <v>41641</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="C31" s="1"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="1"/>
+      <c r="D31" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="32" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="2"/>
-      <c r="B32" s="1"/>
+      <c r="A32" s="5">
+        <v>41642</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="C32" s="1"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="1"/>
+      <c r="D32" s="2">
+        <v>2</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>

</xml_diff>